<commit_message>
Feb 8th all files updated from bala, check for super class
</commit_message>
<xml_diff>
--- a/test_data/open_emr_data.xlsx
+++ b/test_data/open_emr_data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASATEESH\PycharmProjects\HybridFramework\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D0EFC6-E445-4FBE-BBC4-70E23A69B957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E52CE08-D9BE-4CA5-8C6C-60B82EDEC5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{BCDA8807-ED81-472F-9847-535AFA73F269}"/>
   </bookViews>
   <sheets>
-    <sheet name="valid_login" sheetId="1" r:id="rId1"/>
-    <sheet name="invalid_login" sheetId="2" r:id="rId2"/>
+    <sheet name="test_valid_login" sheetId="1" r:id="rId1"/>
+    <sheet name="test_invalid_login" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -492,7 +492,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>